<commit_message>
operations handling changed and home/login css updated
</commit_message>
<xml_diff>
--- a/web/files/excel_calculators_tmp/12c6fc06c99a462375eeb3f43dfd832b08ca9e17.xlsx
+++ b/web/files/excel_calculators_tmp/12c6fc06c99a462375eeb3f43dfd832b08ca9e17.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="72">
   <si>
     <t>Persoon</t>
   </si>
@@ -48,7 +48,7 @@
     <t>Ruben Hazenbosch</t>
   </si>
   <si>
-    <t>Vrouw</t>
+    <t>Man</t>
   </si>
   <si>
     <t>Soort</t>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t>Tot Datum</t>
+  </si>
+  <si>
+    <t>Woonlasten</t>
+  </si>
+  <si>
+    <t>15-06-2012</t>
+  </si>
+  <si>
+    <t>30-09-2053</t>
   </si>
   <si>
     <t>Vervoer</t>
@@ -667,7 +676,7 @@
   <dimension ref="A1:AMK25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1909,7 +1918,7 @@
   <dimension ref="A1:AMK33"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2955,7 +2964,20 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:1025" customHeight="1" ht="12.75"/>
+    <row r="3" spans="1:1025" customHeight="1" ht="12.75">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>450</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="4" spans="1:1025" customHeight="1" ht="12.75"/>
     <row r="5" spans="1:1025" customHeight="1" ht="12.75"/>
     <row r="6" spans="1:1025" customHeight="1" ht="12.75">
@@ -3072,7 +3094,7 @@
     </row>
     <row r="28" spans="1:1025" customHeight="1" ht="12.75">
       <c r="A28" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B28">
         <v>300</v>
@@ -3080,7 +3102,7 @@
     </row>
     <row r="29" spans="1:1025" customHeight="1" ht="12.75">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B29">
         <v>400</v>
@@ -3088,18 +3110,18 @@
     </row>
     <row r="30" spans="1:1025" customHeight="1" ht="12.75">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B30">
         <v>900</v>
       </c>
       <c r="D30" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:1025" customHeight="1" ht="12.75">
       <c r="A31" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B31">
         <v>330</v>
@@ -3107,7 +3129,7 @@
     </row>
     <row r="32" spans="1:1025" customHeight="1" ht="12.75">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B32">
         <v>440</v>
@@ -3115,13 +3137,13 @@
     </row>
     <row r="33" spans="1:1025" customHeight="1" ht="12.75">
       <c r="A33" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B33">
         <v>990</v>
       </c>
       <c r="D33" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -3148,7 +3170,7 @@
   <dimension ref="A1:AMK16"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4182,35 +4204,36 @@
   <sheetData>
     <row r="2" spans="1:1025" customHeight="1" ht="12.75">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:1025" customHeight="1" ht="12.75">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B3" s="5" t="str">
         <f>'Input Oud'!B3</f>
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:1025" customHeight="1" ht="12.75">
       <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="5">
-        <v>30.9111</v>
+        <v>25</v>
+      </c>
+      <c r="B4" s="5" t="str">
+        <f>YEAR('Input Oud'!B19)-YEAR('Input Oud'!B4)+(MONTH('Input Oud'!B19)-MONTH('Input Oud'!B4))/12</f>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:1025" customHeight="1" ht="12.75">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B5" s="5">
         <v>67</v>
@@ -4218,7 +4241,7 @@
     </row>
     <row r="6" spans="1:1025" customHeight="1" ht="12.75">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B6" s="5">
         <v>20</v>
@@ -4226,7 +4249,7 @@
     </row>
     <row r="7" spans="1:1025" customHeight="1" ht="12.75">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B7" s="5">
         <v>450</v>
@@ -4234,7 +4257,7 @@
     </row>
     <row r="8" spans="1:1025" customHeight="1" ht="12.75">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B8" s="5">
         <v>1082</v>
@@ -4242,7 +4265,7 @@
     </row>
     <row r="9" spans="1:1025" customHeight="1" ht="12.75">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B9" s="5" t="str">
         <f>'Input Oud'!B12-(YEAR('Input Oud'!B19)-YEAR('Input Oud'!B11)+(MONTH('Input Oud'!B19)-MONTH('Input Oud'!B11))/12)</f>
@@ -4251,21 +4274,21 @@
     </row>
     <row r="11" spans="1:1025" customHeight="1" ht="12.75">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:1025" customHeight="1" ht="12.75">
       <c r="A12" s="6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:1025" customHeight="1" ht="12.75">
@@ -4282,7 +4305,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:1025" customHeight="1" ht="12.75">
@@ -4299,7 +4322,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:1025" customHeight="1" ht="12.75">
@@ -4316,7 +4339,7 @@
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:1025" customHeight="1" ht="12.75">
@@ -4333,7 +4356,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -5394,7 +5417,7 @@
   <sheetData>
     <row r="3" spans="1:1025" customHeight="1" ht="12.95">
       <c r="A3" s="7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B3" s="8">
         <v>18202</v>
@@ -5405,7 +5428,7 @@
     </row>
     <row r="4" spans="1:1025" customHeight="1" ht="12.95">
       <c r="A4" s="9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B4" s="8">
         <v>18536</v>
@@ -5416,7 +5439,7 @@
     </row>
     <row r="5" spans="1:1025" customHeight="1" ht="12.95">
       <c r="A5" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B5" s="8">
         <v>18810</v>
@@ -5427,7 +5450,7 @@
     </row>
     <row r="6" spans="1:1025" customHeight="1" ht="12.95">
       <c r="A6" s="9" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B6" s="8">
         <v>19085</v>
@@ -5438,7 +5461,7 @@
     </row>
     <row r="7" spans="1:1025" customHeight="1" ht="12.95">
       <c r="A7" s="7" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B7" s="8">
         <v>19359</v>
@@ -5449,7 +5472,7 @@
     </row>
     <row r="8" spans="1:1025" customHeight="1" ht="12.95">
       <c r="A8" s="9" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B8" s="8">
         <v>19603</v>
@@ -5460,7 +5483,7 @@
     </row>
     <row r="9" spans="1:1025" customHeight="1" ht="12.95">
       <c r="A9" s="7" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B9" s="8">
         <v>19845</v>
@@ -5471,7 +5494,7 @@
     </row>
     <row r="10" spans="1:1025" customHeight="1" ht="12.95">
       <c r="A10" s="9" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B10" s="8">
         <v>43831</v>
@@ -5482,32 +5505,32 @@
     </row>
     <row r="11" spans="1:1025" customHeight="1" ht="12.95">
       <c r="A11" s="7" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:1025" customHeight="1" ht="12.95">
       <c r="A12" s="9" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:1025" customHeight="1" ht="12.95">
       <c r="A13" s="7" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:1025" customHeight="1" ht="12.95">
       <c r="A14" s="9" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:1025" customHeight="1" ht="12.95">
       <c r="A15" s="7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:1025" customHeight="1" ht="12.95">
       <c r="A16" s="9" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -6573,19 +6596,19 @@
     </row>
     <row r="2" spans="1:1025" customHeight="1" ht="12.75">
       <c r="A2" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:1025" customHeight="1" ht="12.75">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:1025" customHeight="1" ht="12.75">
@@ -6600,7 +6623,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:1025" customHeight="1" ht="12.75">
@@ -6608,113 +6631,114 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C5" s="11" t="str">
         <f>IF(OR(B5="M",B5="V",B5="onbekend"),"","Geslacht is M, V of onbekend")</f>
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:1025" customHeight="1" ht="12.75">
       <c r="A6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" s="5">
-        <v>46.5</v>
+        <v>60</v>
+      </c>
+      <c r="B6" s="5" t="str">
+        <f>2016-YEAR(B4)+(8-MONTH(B4))/12+(1-DAY(B4))/365</f>
+        <v>0</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="8" spans="1:1025" customHeight="1" ht="12.75">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:1025" customHeight="1" ht="12.75">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:1025" customHeight="1" ht="12.75">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:1025" customHeight="1" ht="12.75">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:1025" customHeight="1" ht="12.75">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:1025" customHeight="1" ht="12.75">
       <c r="A15" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:1025" customHeight="1" ht="12.75">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:1025" customHeight="1" ht="12.75">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:1025" customHeight="1" ht="12.75">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
documents can be uploaded
</commit_message>
<xml_diff>
--- a/web/files/excel_calculators_tmp/12c6fc06c99a462375eeb3f43dfd832b08ca9e17.xlsx
+++ b/web/files/excel_calculators_tmp/12c6fc06c99a462375eeb3f43dfd832b08ca9e17.xlsx
@@ -42,7 +42,7 @@
     <t>Studerend</t>
   </si>
   <si>
-    <t>20-05-1935</t>
+    <t>20-05-1986</t>
   </si>
   <si>
     <t>Ruben Hazenbosch</t>
@@ -667,7 +667,7 @@
   <dimension ref="A1:AMK25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3148,7 +3148,7 @@
   <dimension ref="A1:AMK16"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5535,7 +5535,7 @@
   <dimension ref="A1:AMK19"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6713,7 +6713,9 @@
       <c r="A19" t="s">
         <v>68</v>
       </c>
-      <c r="B19" s="10"/>
+      <c r="B19" s="10">
+        <v>42625</v>
+      </c>
       <c r="C19" s="10"/>
       <c r="D19" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
screen factory operations css updated
</commit_message>
<xml_diff>
--- a/web/files/excel_calculators_tmp/12c6fc06c99a462375eeb3f43dfd832b08ca9e17.xlsx
+++ b/web/files/excel_calculators_tmp/12c6fc06c99a462375eeb3f43dfd832b08ca9e17.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
   <si>
     <t>Persoon</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>Man</t>
+  </si>
+  <si>
+    <t>Partner</t>
+  </si>
+  <si>
+    <t>fghfh</t>
   </si>
   <si>
     <t>Inkomen</t>
@@ -192,7 +198,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
+  </numFmts>
   <fonts count="5">
     <font>
       <b val="0"/>
@@ -302,7 +310,7 @@
     <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="14" fillId="3" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="0">
+    <xf xfId="0" fontId="0" numFmtId="164" fillId="3" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0">
@@ -326,13 +334,13 @@
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="14" fillId="2" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
+    <xf xfId="0" fontId="0" numFmtId="164" fillId="2" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="14" fillId="3" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="0">
+    <xf xfId="0" fontId="0" numFmtId="164" fillId="3" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="14" fillId="2" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
+    <xf xfId="0" fontId="0" numFmtId="164" fillId="2" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
@@ -649,7 +657,7 @@
   <dimension ref="A1:AMK50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1723,11 +1731,21 @@
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:1025">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="4"/>
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="F4" s="5"/>
       <c r="I4" s="6"/>
     </row>
@@ -1901,7 +1919,7 @@
     </row>
     <row r="28" spans="1:1025">
       <c r="A28" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:1025" s="1" customFormat="1">
@@ -1909,19 +1927,19 @@
         <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:1025">
@@ -2113,181 +2131,161 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:5">
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5">
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:5">
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:5">
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:5">
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:5">
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:5">
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:5">
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:5">
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:5">
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:5">
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:5">
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:5">
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5">
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5">
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="1:5">
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:4">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:5">
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5">
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="1:5">
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="1:5">
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:4">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -2331,18 +2329,18 @@
   <sheetData>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B3" s="9" t="str">
         <f>LOOKUP("Kostwinnaar",Input!A3:F25,Input!C3:C25)</f>
@@ -2353,13 +2351,13 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G3" s="11"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B4" s="12" t="str">
         <f>LOOKUP("Kostwinnaar",Input!A3:F25,Input!B3:B25)</f>
@@ -2370,13 +2368,13 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G4" s="11"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B5" s="9" t="str">
         <f>YEAR(instellingen!B2)-YEAR(B4)+(MONTH(instellingen!B2)-MONTH(B4))/12</f>
@@ -2387,12 +2385,12 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B6" s="9" t="str">
         <f>VLOOKUP(B4,instellingen!B4:C11,2)</f>
@@ -2403,12 +2401,12 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B7" s="9">
         <v>20</v>
@@ -2417,7 +2415,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B8" s="9">
         <v>450</v>
@@ -2426,7 +2424,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B9" s="9">
         <v>1082</v>
@@ -2435,7 +2433,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B10" s="9">
         <v>15</v>
@@ -2444,21 +2442,21 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2473,7 +2471,7 @@
         <v>#REF!</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -2487,7 +2485,7 @@
         <v>#REF!</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -2503,7 +2501,7 @@
         <v>#REF!</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -2519,7 +2517,7 @@
         <v>#REF!</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2556,7 +2554,7 @@
   <sheetData>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B2" s="11" t="str">
         <f>TODAY()</f>
@@ -2565,7 +2563,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="16" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B4" s="11">
         <v>18202</v>
@@ -2576,7 +2574,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B5" s="11">
         <v>18536</v>
@@ -2587,7 +2585,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="16" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B6" s="11">
         <v>18810</v>
@@ -2598,7 +2596,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="17" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B7" s="11">
         <v>19085</v>
@@ -2609,7 +2607,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B8" s="11">
         <v>19359</v>
@@ -2620,7 +2618,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B9" s="11">
         <v>19603</v>
@@ -2631,7 +2629,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="16" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B10" s="11">
         <v>19845</v>
@@ -2642,7 +2640,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="17" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B11" s="11">
         <v>43831</v>
@@ -2653,32 +2651,32 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="16" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="17" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="16" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="16" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="17" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>